<commit_message>
Finished first implementation of column header tree
</commit_message>
<xml_diff>
--- a/documents/Example_Table.xlsx
+++ b/documents/Example_Table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielsindlinger/Documents/Uni/Masterarbeit/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{347588CF-EC24-314F-AFC2-A21089C49DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45BD69F6-B4D2-8F4B-B0D4-964F81369A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="980" yWindow="1240" windowWidth="27840" windowHeight="16340" xr2:uid="{5464F0E8-CF65-764F-9830-80FF0E5FA323}"/>
   </bookViews>
@@ -84,7 +84,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -107,29 +107,58 @@
       <family val="1"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Georgia"/>
       <family val="1"/>
     </font>
     <font>
-      <i/>
+      <sz val="18"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Georgia"/>
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF838383"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -137,11 +166,215 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -149,23 +382,80 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -501,10 +791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58328139-2960-C54A-ABB3-ACBBAFEAE705}">
-  <dimension ref="A2:G7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD7"/>
+      <selection activeCell="C6" sqref="C5:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -512,126 +802,135 @@
     <col min="1" max="1" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="5" t="s">
+    <row r="1" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
     </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="5">
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="24" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="23">
         <v>2023</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="6">
+      <c r="E2" s="24"/>
+      <c r="F2" s="23">
         <v>2024</v>
       </c>
-      <c r="G3" s="6"/>
+      <c r="G2" s="25"/>
     </row>
-    <row r="4" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+    <row r="3" spans="1:7" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G3" s="11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+    <row r="4" spans="1:7" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C4" s="14">
         <v>17</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E4" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G4" s="15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
-      <c r="B6" s="2" t="s">
+    <row r="5" spans="1:7" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="27"/>
+      <c r="B5" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C5" s="17">
         <v>16</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F5" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G5" s="18" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="20">
+        <v>17</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="2">
-        <v>17</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="A7" s="4"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="A4:A5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>